<commit_message>
more for 2 sensors
</commit_message>
<xml_diff>
--- a/distanceSensor_table_exel.xlsx
+++ b/distanceSensor_table_exel.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">настоящие см </t>
   </si>
@@ -29,25 +29,13 @@
   <si>
     <t>см в пересчете</t>
   </si>
-  <si>
-    <t>Сумма</t>
-  </si>
-  <si>
-    <t>Среднее</t>
-  </si>
-  <si>
-    <t>С нарастающим итогом</t>
-  </si>
-  <si>
-    <t>Количество</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00_ ;[Red]\-0.00\ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -81,7 +69,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -100,7 +88,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -183,6 +171,21 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Аркуш1!$B$2:$B$22</c:f>
@@ -328,7 +331,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000015-3ED1-469A-863F-5BD91A67B05D}"/>
             </c:ext>
@@ -342,11 +345,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="477939664"/>
-        <c:axId val="477940080"/>
+        <c:axId val="207707440"/>
+        <c:axId val="207710576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="477939664"/>
+        <c:axId val="207707440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,8 +376,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -397,12 +401,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477940080"/>
+        <c:crossAx val="207710576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="477940080"/>
+        <c:axId val="207710576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +462,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477939664"/>
+        <c:crossAx val="207707440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1389,16 +1393,16 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C22"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>9.5</v>
       </c>
@@ -1420,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>15</v>
       </c>
@@ -1432,7 +1436,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22</v>
       </c>
@@ -1443,7 +1447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>28</v>
       </c>
@@ -1454,7 +1458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>34</v>
       </c>
@@ -1465,7 +1469,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>39</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>45</v>
       </c>
@@ -1487,7 +1491,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>54</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>59</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>61.7</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>65.5</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>66</v>
       </c>
@@ -1542,7 +1546,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>70</v>
       </c>
@@ -1553,7 +1557,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>73</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>78.5</v>
       </c>
@@ -1575,7 +1579,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>86.5</v>
       </c>
@@ -1586,7 +1590,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>93.2</v>
       </c>
@@ -1597,7 +1601,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>100</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>170</v>
       </c>
@@ -1619,7 +1623,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>232</v>
       </c>
@@ -1630,7 +1634,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>320</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>380</v>
       </c>

</xml_diff>